<commit_message>
solo esta en prueba
</commit_message>
<xml_diff>
--- a/presupuesto.xlsx
+++ b/presupuesto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Desktop\P3_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332D69CA-7B00-43A4-8CE1-4C7D9FAADF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5780E957-8FC6-4197-B638-91C835B220CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <r>
       <rPr>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -876,8 +876,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>6</v>
+      <c r="A26" s="12">
+        <v>45738</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="11"/>

</xml_diff>